<commit_message>
added check for check function
</commit_message>
<xml_diff>
--- a/ChessEngineTruboCabla/BoardVisuals/ChessBoard120.xlsx
+++ b/ChessEngineTruboCabla/BoardVisuals/ChessBoard120.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\source\repos\ChessEngineTruboCabla\ChessEngineTruboCabla\BoardVisuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{4DF58CB6-2725-4955-BF82-76F24D064D37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{1B865226-E058-47F6-A8EC-75100179ED1C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA81D803-670F-4D10-933F-A7001EDE2B03}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38040" yWindow="1395" windowWidth="27090" windowHeight="12630" xr2:uid="{97CAB0FD-2180-4824-9680-971BCB9BAB55}"/>
+    <workbookView xWindow="570" yWindow="3390" windowWidth="27090" windowHeight="13170" xr2:uid="{97CAB0FD-2180-4824-9680-971BCB9BAB55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -64,6 +64,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -95,12 +107,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -419,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8C40C0-E64A-4A21-9C28-032CB3B15629}">
   <dimension ref="D2:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -588,7 +606,7 @@
       <c r="T5" s="2">
         <v>11</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="4">
         <v>12</v>
       </c>
       <c r="V5" s="2">
@@ -694,16 +712,16 @@
       <c r="R7" s="2">
         <v>25</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="4">
         <v>26</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="4">
         <v>27</v>
       </c>
       <c r="U7" s="2">
         <v>28</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7" s="4">
         <v>29</v>
       </c>
       <c r="W7" s="2">
@@ -756,7 +774,7 @@
       <c r="T8" s="2">
         <v>35</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="3">
         <v>36</v>
       </c>
       <c r="V8" s="2">
@@ -765,7 +783,7 @@
       <c r="W8" s="2">
         <v>38</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8" s="4">
         <v>39</v>
       </c>
     </row>
@@ -874,7 +892,7 @@
       <c r="V10" s="2">
         <v>53</v>
       </c>
-      <c r="W10" s="2">
+      <c r="W10" s="4">
         <v>54</v>
       </c>
       <c r="X10" s="2">

</xml_diff>